<commit_message>
add stats vs Mopogo Males
</commit_message>
<xml_diff>
--- a/public/statistic/teams-raiting.xlsx
+++ b/public/statistic/teams-raiting.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Баскетбол\Отчёты\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0D9597F0-6EB9-4666-A6FF-E60F605F684C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F0C146E9-AA71-4082-B86A-229CDB0B3B56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8880" xr2:uid="{EC81D871-1906-46FC-AF98-2FE79519B3C1}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8880" xr2:uid="{5A5CA3A5-E5FB-484C-BFEE-CF6C71F1A56D}"/>
   </bookViews>
   <sheets>
     <sheet name="Рейтинг команд" sheetId="1" r:id="rId1"/>
@@ -553,7 +553,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61A3DF69-10E4-4988-A768-ADB482C40AC2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{858AC734-0ED3-4B6B-BECF-9A85AAB48492}">
   <dimension ref="A1:O118"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -636,10 +636,10 @@
         <v>1</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="G3" s="3">
-        <v>189.6</v>
+        <v>189.4</v>
       </c>
       <c r="I3" s="3">
         <v>1</v>
@@ -659,16 +659,16 @@
         <v>4</v>
       </c>
       <c r="C4" s="3">
-        <v>40.799999999999997</v>
+        <v>40.9</v>
       </c>
       <c r="E4" s="3">
         <v>2</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G4" s="3">
-        <v>189.4</v>
+        <v>189</v>
       </c>
       <c r="I4" s="3">
         <v>2</v>
@@ -688,16 +688,16 @@
         <v>5</v>
       </c>
       <c r="C5" s="3">
-        <v>35.299999999999997</v>
+        <v>36.1</v>
       </c>
       <c r="E5" s="3">
         <v>3</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="G5" s="3">
-        <v>189.3</v>
+        <v>189</v>
       </c>
       <c r="I5" s="3">
         <v>3</v>
@@ -717,16 +717,16 @@
         <v>6</v>
       </c>
       <c r="C6" s="3">
-        <v>34.4</v>
+        <v>34.5</v>
       </c>
       <c r="E6" s="3">
         <v>4</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="G6" s="3">
-        <v>189.1</v>
+        <v>188.8</v>
       </c>
       <c r="I6" s="3">
         <v>4</v>
@@ -752,10 +752,10 @@
         <v>5</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="G7" s="3">
-        <v>188.8</v>
+        <v>188.2</v>
       </c>
       <c r="I7" s="3">
         <v>5</v>
@@ -781,10 +781,10 @@
         <v>6</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="G8" s="3">
-        <v>188.2</v>
+        <v>188.1</v>
       </c>
       <c r="I8" s="3">
         <v>6</v>
@@ -793,7 +793,7 @@
         <v>4</v>
       </c>
       <c r="K8" s="3">
-        <v>86.4</v>
+        <v>85.9</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -810,10 +810,10 @@
         <v>7</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="G9" s="3">
-        <v>188.1</v>
+        <v>188</v>
       </c>
       <c r="I9" s="3">
         <v>7</v>
@@ -833,16 +833,16 @@
         <v>10</v>
       </c>
       <c r="C10" s="3">
-        <v>29.6</v>
+        <v>29.7</v>
       </c>
       <c r="E10" s="3">
         <v>8</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G10" s="3">
-        <v>188</v>
+        <v>187.9</v>
       </c>
       <c r="I10" s="3">
         <v>8</v>
@@ -851,7 +851,7 @@
         <v>11</v>
       </c>
       <c r="K10" s="3">
-        <v>84.6</v>
+        <v>84.3</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -862,7 +862,7 @@
         <v>11</v>
       </c>
       <c r="C11" s="3">
-        <v>27.8</v>
+        <v>27.5</v>
       </c>
       <c r="E11" s="3">
         <v>9</v>
@@ -877,10 +877,10 @@
         <v>9</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="K11" s="3">
-        <v>83.4</v>
+        <v>82.1</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -897,19 +897,19 @@
         <v>10</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G12" s="3">
-        <v>185.8</v>
+        <v>185.6</v>
       </c>
       <c r="I12" s="3">
         <v>10</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="K12" s="3">
-        <v>81.099999999999994</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -926,19 +926,19 @@
         <v>11</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G13" s="3">
-        <v>185.6</v>
+        <v>185.3</v>
       </c>
       <c r="I13" s="3">
         <v>11</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="K13" s="3">
-        <v>80.599999999999994</v>
+        <v>81.099999999999994</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -949,16 +949,16 @@
         <v>14</v>
       </c>
       <c r="C14" s="3">
-        <v>16.8</v>
+        <v>17.8</v>
       </c>
       <c r="E14" s="3">
         <v>12</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="G14" s="3">
-        <v>185.3</v>
+        <v>184.6</v>
       </c>
       <c r="I14" s="3">
         <v>12</v>
@@ -967,7 +967,7 @@
         <v>16</v>
       </c>
       <c r="K14" s="3">
-        <v>80.3</v>
+        <v>80.599999999999994</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -978,16 +978,16 @@
         <v>15</v>
       </c>
       <c r="C15" s="3">
-        <v>15.7</v>
+        <v>15.8</v>
       </c>
       <c r="E15" s="3">
         <v>13</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="G15" s="3">
-        <v>183.5</v>
+        <v>184.5</v>
       </c>
       <c r="I15" s="3">
         <v>13</v>
@@ -996,7 +996,7 @@
         <v>15</v>
       </c>
       <c r="K15" s="3">
-        <v>79.8</v>
+        <v>79.5</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -1007,7 +1007,7 @@
         <v>16</v>
       </c>
       <c r="C16" s="3">
-        <v>12.4</v>
+        <v>13.9</v>
       </c>
       <c r="E16" s="3">
         <v>14</v>
@@ -1065,7 +1065,7 @@
         <v>1</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C20" s="3">
         <v>0</v>
@@ -1074,7 +1074,7 @@
         <v>1</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="G20" s="5">
         <v>0.8</v>
@@ -1085,7 +1085,7 @@
         <v>2</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C21" s="3">
         <v>0</v>
@@ -1097,7 +1097,7 @@
         <v>3</v>
       </c>
       <c r="G21" s="5">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
@@ -1114,10 +1114,10 @@
         <v>3</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="G22" s="5">
-        <v>0.73</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
@@ -1125,7 +1125,7 @@
         <v>4</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C23" s="3">
         <v>0</v>
@@ -1134,10 +1134,10 @@
         <v>4</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="G23" s="5">
-        <v>0.7</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
@@ -1154,7 +1154,7 @@
         <v>5</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="G24" s="5">
         <v>0.6</v>
@@ -1174,10 +1174,10 @@
         <v>6</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G25" s="5">
-        <v>0.6</v>
+        <v>0.56000000000000005</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
@@ -1194,10 +1194,10 @@
         <v>7</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G26" s="5">
-        <v>0.6</v>
+        <v>0.53</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
@@ -1217,7 +1217,7 @@
         <v>4</v>
       </c>
       <c r="G27" s="5">
-        <v>0.5</v>
+        <v>0.47</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
@@ -1234,10 +1234,10 @@
         <v>9</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G28" s="5">
-        <v>0.45</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
@@ -1254,7 +1254,7 @@
         <v>10</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G29" s="5">
         <v>0.4</v>
@@ -1274,7 +1274,7 @@
         <v>11</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="G30" s="5">
         <v>0.4</v>
@@ -1294,10 +1294,10 @@
         <v>12</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="G31" s="5">
-        <v>0.4</v>
+        <v>0.38</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
@@ -1314,10 +1314,10 @@
         <v>13</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="G32" s="5">
-        <v>0.3</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.3">
@@ -1337,7 +1337,7 @@
         <v>14</v>
       </c>
       <c r="G33" s="5">
-        <v>0</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.3">
@@ -1405,10 +1405,10 @@
         <v>1</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C37" s="3">
-        <v>81</v>
+        <v>80.3</v>
       </c>
       <c r="E37" s="3">
         <v>1</v>
@@ -1417,7 +1417,7 @@
         <v>15</v>
       </c>
       <c r="G37" s="3">
-        <v>45.5</v>
+        <v>46.7</v>
       </c>
       <c r="I37" s="3">
         <v>1</v>
@@ -1426,16 +1426,16 @@
         <v>12</v>
       </c>
       <c r="K37" s="3">
-        <v>51.5</v>
+        <v>52.7</v>
       </c>
       <c r="M37" s="3">
         <v>1</v>
       </c>
       <c r="N37" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="O37" s="3">
-        <v>16</v>
+        <v>16.7</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.3">
@@ -1443,19 +1443,19 @@
         <v>2</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C38" s="3">
-        <v>78.5</v>
+        <v>79</v>
       </c>
       <c r="E38" s="3">
         <v>2</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G38" s="3">
-        <v>57</v>
+        <v>51.3</v>
       </c>
       <c r="I38" s="3">
         <v>2</v>
@@ -1464,16 +1464,16 @@
         <v>4</v>
       </c>
       <c r="K38" s="3">
-        <v>48.5</v>
+        <v>49.3</v>
       </c>
       <c r="M38" s="3">
         <v>2</v>
       </c>
       <c r="N38" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="O38" s="3">
-        <v>16</v>
+        <v>16.7</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.3">
@@ -1481,19 +1481,19 @@
         <v>3</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C39" s="3">
-        <v>74</v>
+        <v>77.7</v>
       </c>
       <c r="E39" s="3">
         <v>3</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="G39" s="3">
-        <v>57.5</v>
+        <v>57</v>
       </c>
       <c r="I39" s="3">
         <v>3</v>
@@ -1502,16 +1502,16 @@
         <v>3</v>
       </c>
       <c r="K39" s="3">
-        <v>48</v>
+        <v>48.5</v>
       </c>
       <c r="M39" s="3">
         <v>3</v>
       </c>
       <c r="N39" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O39" s="3">
-        <v>15.5</v>
+        <v>14.7</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.3">
@@ -1519,37 +1519,37 @@
         <v>4</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C40" s="3">
-        <v>71.5</v>
+        <v>69.7</v>
       </c>
       <c r="E40" s="3">
         <v>4</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="G40" s="3">
-        <v>58</v>
+        <v>57.7</v>
       </c>
       <c r="I40" s="3">
         <v>4</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="K40" s="3">
-        <v>48</v>
+        <v>47.3</v>
       </c>
       <c r="M40" s="3">
         <v>4</v>
       </c>
       <c r="N40" s="4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="O40" s="3">
-        <v>15.5</v>
+        <v>14.3</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.3">
@@ -1557,34 +1557,34 @@
         <v>5</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C41" s="3">
-        <v>69.5</v>
+        <v>66.3</v>
       </c>
       <c r="E41" s="3">
         <v>5</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="G41" s="3">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I41" s="3">
         <v>5</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="K41" s="3">
-        <v>46</v>
+        <v>46.7</v>
       </c>
       <c r="M41" s="3">
         <v>5</v>
       </c>
       <c r="N41" s="4" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="O41" s="3">
         <v>14</v>
@@ -1595,34 +1595,34 @@
         <v>6</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C42" s="3">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E42" s="3">
         <v>6</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G42" s="3">
-        <v>60</v>
+        <v>59.5</v>
       </c>
       <c r="I42" s="3">
         <v>6</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="K42" s="3">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M42" s="3">
         <v>6</v>
       </c>
       <c r="N42" s="4" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="O42" s="3">
         <v>13.5</v>
@@ -1636,34 +1636,34 @@
         <v>7</v>
       </c>
       <c r="C43" s="3">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E43" s="3">
         <v>7</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G43" s="3">
-        <v>60.5</v>
+        <v>63.7</v>
       </c>
       <c r="I43" s="3">
         <v>7</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="K43" s="3">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M43" s="3">
         <v>7</v>
       </c>
       <c r="N43" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O43" s="3">
-        <v>12.5</v>
+        <v>13.3</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.3">
@@ -1671,37 +1671,37 @@
         <v>8</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C44" s="3">
-        <v>61.5</v>
+        <v>62.3</v>
       </c>
       <c r="E44" s="3">
         <v>8</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="G44" s="3">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I44" s="3">
         <v>8</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="K44" s="3">
-        <v>44.5</v>
+        <v>43</v>
       </c>
       <c r="M44" s="3">
         <v>8</v>
       </c>
       <c r="N44" s="4" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="O44" s="3">
-        <v>12.5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.3">
@@ -1709,16 +1709,16 @@
         <v>9</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C45" s="3">
-        <v>58.5</v>
+        <v>62</v>
       </c>
       <c r="E45" s="3">
         <v>9</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G45" s="3">
         <v>64</v>
@@ -1727,19 +1727,19 @@
         <v>9</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="K45" s="3">
-        <v>42</v>
+        <v>42.3</v>
       </c>
       <c r="M45" s="3">
         <v>9</v>
       </c>
       <c r="N45" s="4" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="O45" s="3">
-        <v>12</v>
+        <v>12.7</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.3">
@@ -1747,28 +1747,28 @@
         <v>10</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C46" s="3">
-        <v>56.5</v>
+        <v>57.3</v>
       </c>
       <c r="E46" s="3">
         <v>10</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G46" s="3">
-        <v>64.5</v>
+        <v>64</v>
       </c>
       <c r="I46" s="3">
         <v>10</v>
       </c>
       <c r="J46" s="4" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="K46" s="3">
-        <v>41</v>
+        <v>41.7</v>
       </c>
       <c r="M46" s="3">
         <v>10</v>
@@ -1777,7 +1777,7 @@
         <v>11</v>
       </c>
       <c r="O46" s="3">
-        <v>11</v>
+        <v>12.7</v>
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.3">
@@ -1788,31 +1788,31 @@
         <v>9</v>
       </c>
       <c r="C47" s="3">
-        <v>56.5</v>
+        <v>56.7</v>
       </c>
       <c r="E47" s="3">
         <v>11</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G47" s="3">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="I47" s="3">
         <v>11</v>
       </c>
       <c r="J47" s="4" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="K47" s="3">
-        <v>39</v>
+        <v>40.700000000000003</v>
       </c>
       <c r="M47" s="3">
         <v>11</v>
       </c>
       <c r="N47" s="4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="O47" s="3">
         <v>10</v>
@@ -1823,19 +1823,19 @@
         <v>12</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C48" s="3">
-        <v>56.5</v>
+        <v>54</v>
       </c>
       <c r="E48" s="3">
         <v>12</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="G48" s="3">
-        <v>68.5</v>
+        <v>68</v>
       </c>
       <c r="I48" s="3">
         <v>12</v>
@@ -1844,16 +1844,16 @@
         <v>16</v>
       </c>
       <c r="K48" s="3">
-        <v>37.5</v>
+        <v>37</v>
       </c>
       <c r="M48" s="3">
         <v>12</v>
       </c>
       <c r="N48" s="4" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="O48" s="3">
-        <v>9</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.3">
@@ -1864,7 +1864,7 @@
         <v>3</v>
       </c>
       <c r="C49" s="3">
-        <v>51</v>
+        <v>50.5</v>
       </c>
       <c r="E49" s="3">
         <v>13</v>
@@ -1873,7 +1873,7 @@
         <v>14</v>
       </c>
       <c r="G49" s="3">
-        <v>75</v>
+        <v>72.5</v>
       </c>
       <c r="I49" s="3">
         <v>13</v>
@@ -1882,16 +1882,16 @@
         <v>7</v>
       </c>
       <c r="K49" s="3">
-        <v>35.5</v>
+        <v>36.700000000000003</v>
       </c>
       <c r="M49" s="3">
         <v>13</v>
       </c>
       <c r="N49" s="4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="O49" s="3">
-        <v>8</v>
+        <v>9.3000000000000007</v>
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.3">
@@ -1902,7 +1902,7 @@
         <v>16</v>
       </c>
       <c r="C50" s="3">
-        <v>49.5</v>
+        <v>45</v>
       </c>
       <c r="E50" s="3">
         <v>14</v>
@@ -1911,7 +1911,7 @@
         <v>16</v>
       </c>
       <c r="G50" s="3">
-        <v>99.5</v>
+        <v>96.3</v>
       </c>
       <c r="I50" s="3">
         <v>14</v>
@@ -1920,7 +1920,7 @@
         <v>14</v>
       </c>
       <c r="K50" s="3">
-        <v>28</v>
+        <v>35.5</v>
       </c>
       <c r="M50" s="3">
         <v>14</v>
@@ -1929,7 +1929,7 @@
         <v>16</v>
       </c>
       <c r="O50" s="3">
-        <v>7</v>
+        <v>6.7</v>
       </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.3">
@@ -1986,7 +1986,7 @@
         <v>11</v>
       </c>
       <c r="C54" s="3">
-        <v>16.5</v>
+        <v>18</v>
       </c>
       <c r="E54" s="3">
         <v>1</v>
@@ -1995,16 +1995,16 @@
         <v>15</v>
       </c>
       <c r="G54" s="3">
-        <v>5.5</v>
+        <v>6</v>
       </c>
       <c r="I54" s="3">
         <v>1</v>
       </c>
       <c r="J54" s="4" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="K54" s="3">
-        <v>13</v>
+        <v>13.7</v>
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.3">
@@ -2015,7 +2015,7 @@
         <v>13</v>
       </c>
       <c r="C55" s="3">
-        <v>15</v>
+        <v>14.7</v>
       </c>
       <c r="E55" s="3">
         <v>2</v>
@@ -2024,16 +2024,16 @@
         <v>12</v>
       </c>
       <c r="G55" s="3">
-        <v>4.5</v>
+        <v>4.7</v>
       </c>
       <c r="I55" s="3">
         <v>2</v>
       </c>
       <c r="J55" s="4" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="K55" s="3">
-        <v>13.5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.3">
@@ -2044,25 +2044,25 @@
         <v>15</v>
       </c>
       <c r="C56" s="3">
+        <v>14</v>
+      </c>
+      <c r="E56" s="3">
+        <v>3</v>
+      </c>
+      <c r="F56" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G56" s="3">
+        <v>4.3</v>
+      </c>
+      <c r="I56" s="3">
+        <v>3</v>
+      </c>
+      <c r="J56" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K56" s="3">
         <v>14.5</v>
-      </c>
-      <c r="E56" s="3">
-        <v>3</v>
-      </c>
-      <c r="F56" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G56" s="3">
-        <v>4.5</v>
-      </c>
-      <c r="I56" s="3">
-        <v>3</v>
-      </c>
-      <c r="J56" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="K56" s="3">
-        <v>14</v>
       </c>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.3">
@@ -2070,7 +2070,7 @@
         <v>4</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C57" s="3">
         <v>13</v>
@@ -2079,10 +2079,10 @@
         <v>4</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G57" s="3">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="I57" s="3">
         <v>4</v>
@@ -2091,7 +2091,7 @@
         <v>13</v>
       </c>
       <c r="K57" s="3">
-        <v>15.5</v>
+        <v>16</v>
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.3">
@@ -2102,25 +2102,25 @@
         <v>12</v>
       </c>
       <c r="C58" s="3">
-        <v>11</v>
+        <v>12.7</v>
       </c>
       <c r="E58" s="3">
         <v>5</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="G58" s="3">
-        <v>3</v>
+        <v>3.3</v>
       </c>
       <c r="I58" s="3">
         <v>5</v>
       </c>
       <c r="J58" s="4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="K58" s="3">
-        <v>15.5</v>
+        <v>16.3</v>
       </c>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.3">
@@ -2131,25 +2131,25 @@
         <v>6</v>
       </c>
       <c r="C59" s="3">
-        <v>10.5</v>
+        <v>12.3</v>
       </c>
       <c r="E59" s="3">
         <v>6</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="G59" s="3">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="I59" s="3">
         <v>6</v>
       </c>
       <c r="J59" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K59" s="3">
-        <v>16.5</v>
+        <v>17.3</v>
       </c>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.3">
@@ -2160,25 +2160,25 @@
         <v>8</v>
       </c>
       <c r="C60" s="3">
-        <v>9.5</v>
+        <v>10.7</v>
       </c>
       <c r="E60" s="3">
         <v>7</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="G60" s="3">
-        <v>2.5</v>
+        <v>2.7</v>
       </c>
       <c r="I60" s="3">
         <v>7</v>
       </c>
       <c r="J60" s="4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="K60" s="3">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.3">
@@ -2186,28 +2186,28 @@
         <v>8</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C61" s="3">
-        <v>9</v>
+        <v>10.7</v>
       </c>
       <c r="E61" s="3">
         <v>8</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="G61" s="3">
-        <v>2.5</v>
+        <v>2.7</v>
       </c>
       <c r="I61" s="3">
         <v>8</v>
       </c>
       <c r="J61" s="4" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="K61" s="3">
-        <v>17</v>
+        <v>18.3</v>
       </c>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.3">
@@ -2215,10 +2215,10 @@
         <v>9</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C62" s="3">
-        <v>8</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="E62" s="3">
         <v>9</v>
@@ -2227,16 +2227,16 @@
         <v>13</v>
       </c>
       <c r="G62" s="3">
-        <v>2</v>
+        <v>2.7</v>
       </c>
       <c r="I62" s="3">
         <v>9</v>
       </c>
       <c r="J62" s="4" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="K62" s="3">
-        <v>20</v>
+        <v>19.7</v>
       </c>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.3">
@@ -2247,25 +2247,25 @@
         <v>14</v>
       </c>
       <c r="C63" s="3">
-        <v>8</v>
+        <v>8.5</v>
       </c>
       <c r="E63" s="3">
         <v>10</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="G63" s="3">
-        <v>2</v>
+        <v>2.7</v>
       </c>
       <c r="I63" s="3">
         <v>10</v>
       </c>
       <c r="J63" s="4" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="K63" s="3">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.3">
@@ -2273,25 +2273,25 @@
         <v>11</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="C64" s="3">
-        <v>8</v>
+        <v>7.7</v>
       </c>
       <c r="E64" s="3">
         <v>11</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G64" s="3">
-        <v>1</v>
+        <v>1.3</v>
       </c>
       <c r="I64" s="3">
         <v>11</v>
       </c>
       <c r="J64" s="4" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="K64" s="3">
         <v>21</v>
@@ -2305,13 +2305,13 @@
         <v>9</v>
       </c>
       <c r="C65" s="3">
-        <v>7</v>
+        <v>7.7</v>
       </c>
       <c r="E65" s="3">
         <v>12</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G65" s="3">
         <v>1</v>
@@ -2320,10 +2320,10 @@
         <v>12</v>
       </c>
       <c r="J65" s="4" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="K65" s="3">
-        <v>21.5</v>
+        <v>22</v>
       </c>
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.3">
@@ -2334,7 +2334,7 @@
         <v>5</v>
       </c>
       <c r="C66" s="3">
-        <v>6</v>
+        <v>6.3</v>
       </c>
       <c r="E66" s="3">
         <v>13</v>
@@ -2343,16 +2343,16 @@
         <v>7</v>
       </c>
       <c r="G66" s="3">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="I66" s="3">
         <v>13</v>
       </c>
       <c r="J66" s="4" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="K66" s="3">
-        <v>24.5</v>
+        <v>26.7</v>
       </c>
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.3">
@@ -2363,7 +2363,7 @@
         <v>3</v>
       </c>
       <c r="C67" s="3">
-        <v>6</v>
+        <v>5.5</v>
       </c>
       <c r="E67" s="3">
         <v>14</v>
@@ -2372,16 +2372,16 @@
         <v>3</v>
       </c>
       <c r="G67" s="3">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I67" s="3">
         <v>14</v>
       </c>
       <c r="J67" s="4" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="K67" s="3">
-        <v>26.5</v>
+        <v>27</v>
       </c>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.3">
@@ -2452,16 +2452,16 @@
         <v>14</v>
       </c>
       <c r="C71" s="5">
-        <v>0.64</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="E71" s="3">
         <v>1</v>
       </c>
       <c r="F71" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="G71" s="5">
-        <v>0.45</v>
+        <v>0.33</v>
       </c>
       <c r="I71" s="3">
         <v>1</v>
@@ -2470,7 +2470,7 @@
         <v>12</v>
       </c>
       <c r="K71" s="5">
-        <v>0.68</v>
+        <v>0.67</v>
       </c>
       <c r="M71" s="3">
         <v>1</v>
@@ -2479,7 +2479,7 @@
         <v>14</v>
       </c>
       <c r="O71" s="5">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="72" spans="1:15" x14ac:dyDescent="0.3">
@@ -2490,7 +2490,7 @@
         <v>15</v>
       </c>
       <c r="C72" s="5">
-        <v>0.63</v>
+        <v>0.52</v>
       </c>
       <c r="E72" s="3">
         <v>2</v>
@@ -2499,25 +2499,25 @@
         <v>7</v>
       </c>
       <c r="G72" s="5">
-        <v>0.38</v>
+        <v>0.33</v>
       </c>
       <c r="I72" s="3">
         <v>2</v>
       </c>
       <c r="J72" s="4" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="K72" s="5">
-        <v>0.64</v>
+        <v>0.61</v>
       </c>
       <c r="M72" s="3">
         <v>2</v>
       </c>
       <c r="N72" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="O72" s="5">
-        <v>0.45</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="73" spans="1:15" x14ac:dyDescent="0.3">
@@ -2534,10 +2534,10 @@
         <v>3</v>
       </c>
       <c r="F73" s="4" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="G73" s="5">
-        <v>0.37</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="I73" s="3">
         <v>3</v>
@@ -2546,16 +2546,16 @@
         <v>5</v>
       </c>
       <c r="K73" s="5">
-        <v>0.64</v>
+        <v>0.6</v>
       </c>
       <c r="M73" s="3">
         <v>3</v>
       </c>
       <c r="N73" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="O73" s="5">
-        <v>0.38</v>
+        <v>0.39</v>
       </c>
     </row>
     <row r="74" spans="1:15" x14ac:dyDescent="0.3">
@@ -2566,34 +2566,34 @@
         <v>12</v>
       </c>
       <c r="C74" s="5">
-        <v>0.41</v>
+        <v>0.49</v>
       </c>
       <c r="E74" s="3">
         <v>4</v>
       </c>
       <c r="F74" s="4" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="G74" s="5">
-        <v>0.25</v>
+        <v>0.27</v>
       </c>
       <c r="I74" s="3">
         <v>4</v>
       </c>
       <c r="J74" s="4" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="K74" s="5">
-        <v>0.62</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="M74" s="3">
         <v>4</v>
       </c>
       <c r="N74" s="4" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="O74" s="5">
-        <v>0.35</v>
+        <v>0.38</v>
       </c>
     </row>
     <row r="75" spans="1:15" x14ac:dyDescent="0.3">
@@ -2610,7 +2610,7 @@
         <v>5</v>
       </c>
       <c r="F75" s="4" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="G75" s="5">
         <v>0.22</v>
@@ -2619,19 +2619,19 @@
         <v>5</v>
       </c>
       <c r="J75" s="4" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="K75" s="5">
-        <v>0.6</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="M75" s="3">
         <v>5</v>
       </c>
       <c r="N75" s="4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="O75" s="5">
-        <v>0.34</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="76" spans="1:15" x14ac:dyDescent="0.3">
@@ -2639,7 +2639,7 @@
         <v>6</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C76" s="5">
         <v>0.39</v>
@@ -2648,7 +2648,7 @@
         <v>6</v>
       </c>
       <c r="F76" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G76" s="5">
         <v>0.21</v>
@@ -2657,19 +2657,19 @@
         <v>6</v>
       </c>
       <c r="J76" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K76" s="5">
-        <v>0.56000000000000005</v>
+        <v>0.54</v>
       </c>
       <c r="M76" s="3">
         <v>6</v>
       </c>
       <c r="N76" s="4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="O76" s="5">
-        <v>0.33</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="77" spans="1:15" x14ac:dyDescent="0.3">
@@ -2677,7 +2677,7 @@
         <v>7</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C77" s="5">
         <v>0.38</v>
@@ -2686,25 +2686,25 @@
         <v>7</v>
       </c>
       <c r="F77" s="4" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="G77" s="5">
-        <v>0.21</v>
+        <v>0.2</v>
       </c>
       <c r="I77" s="3">
         <v>7</v>
       </c>
       <c r="J77" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="K77" s="5">
-        <v>0.55000000000000004</v>
+        <v>0.54</v>
       </c>
       <c r="M77" s="3">
         <v>7</v>
       </c>
       <c r="N77" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O77" s="5">
         <v>0.33</v>
@@ -2724,16 +2724,16 @@
         <v>8</v>
       </c>
       <c r="F78" s="4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G78" s="5">
-        <v>0.21</v>
+        <v>0.2</v>
       </c>
       <c r="I78" s="3">
         <v>8</v>
       </c>
       <c r="J78" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="K78" s="5">
         <v>0.53</v>
@@ -2742,7 +2742,7 @@
         <v>8</v>
       </c>
       <c r="N78" s="4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="O78" s="5">
         <v>0.33</v>
@@ -2753,10 +2753,10 @@
         <v>9</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C79" s="5">
-        <v>0.37</v>
+        <v>0.36</v>
       </c>
       <c r="E79" s="3">
         <v>9</v>
@@ -2765,7 +2765,7 @@
         <v>12</v>
       </c>
       <c r="G79" s="5">
-        <v>0.21</v>
+        <v>0.19</v>
       </c>
       <c r="I79" s="3">
         <v>9</v>
@@ -2774,16 +2774,16 @@
         <v>4</v>
       </c>
       <c r="K79" s="5">
-        <v>0.51</v>
+        <v>0.52</v>
       </c>
       <c r="M79" s="3">
         <v>9</v>
       </c>
       <c r="N79" s="4" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="O79" s="5">
-        <v>0.33</v>
+        <v>0.32</v>
       </c>
     </row>
     <row r="80" spans="1:15" x14ac:dyDescent="0.3">
@@ -2791,37 +2791,37 @@
         <v>10</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C80" s="5">
-        <v>0.34</v>
+        <v>0.36</v>
       </c>
       <c r="E80" s="3">
         <v>10</v>
       </c>
       <c r="F80" s="4" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="G80" s="5">
-        <v>0.2</v>
+        <v>0.19</v>
       </c>
       <c r="I80" s="3">
         <v>10</v>
       </c>
       <c r="J80" s="4" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="K80" s="5">
-        <v>0.47</v>
+        <v>0.5</v>
       </c>
       <c r="M80" s="3">
         <v>10</v>
       </c>
       <c r="N80" s="4" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="O80" s="5">
-        <v>0.32</v>
+        <v>0.31</v>
       </c>
     </row>
     <row r="81" spans="1:15" x14ac:dyDescent="0.3">
@@ -2829,28 +2829,28 @@
         <v>11</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C81" s="5">
-        <v>0.34</v>
+        <v>0.35</v>
       </c>
       <c r="E81" s="3">
         <v>11</v>
       </c>
       <c r="F81" s="4" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="G81" s="5">
-        <v>0.2</v>
+        <v>0.17</v>
       </c>
       <c r="I81" s="3">
         <v>11</v>
       </c>
       <c r="J81" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K81" s="5">
-        <v>0.42</v>
+        <v>0.46</v>
       </c>
       <c r="M81" s="3">
         <v>11</v>
@@ -2859,7 +2859,7 @@
         <v>8</v>
       </c>
       <c r="O81" s="5">
-        <v>0.3</v>
+        <v>0.31</v>
       </c>
     </row>
     <row r="82" spans="1:15" x14ac:dyDescent="0.3">
@@ -2867,34 +2867,34 @@
         <v>12</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C82" s="5">
-        <v>0.34</v>
+        <v>0.35</v>
       </c>
       <c r="E82" s="3">
         <v>12</v>
       </c>
       <c r="F82" s="4" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="G82" s="5">
-        <v>0.18</v>
+        <v>0.17</v>
       </c>
       <c r="I82" s="3">
         <v>12</v>
       </c>
       <c r="J82" s="4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="K82" s="5">
-        <v>0.42</v>
+        <v>0.45</v>
       </c>
       <c r="M82" s="3">
         <v>12</v>
       </c>
       <c r="N82" s="4" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="O82" s="5">
         <v>0.3</v>
@@ -2905,19 +2905,19 @@
         <v>13</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C83" s="5">
-        <v>0.31</v>
+        <v>0.35</v>
       </c>
       <c r="E83" s="3">
         <v>13</v>
       </c>
       <c r="F83" s="4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G83" s="5">
-        <v>0.14000000000000001</v>
+        <v>0.16</v>
       </c>
       <c r="I83" s="3">
         <v>13</v>
@@ -2926,16 +2926,16 @@
         <v>15</v>
       </c>
       <c r="K83" s="5">
-        <v>0.34</v>
+        <v>0.32</v>
       </c>
       <c r="M83" s="3">
         <v>13</v>
       </c>
       <c r="N83" s="4" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="O83" s="5">
-        <v>0.28999999999999998</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="84" spans="1:15" x14ac:dyDescent="0.3">
@@ -2946,16 +2946,16 @@
         <v>7</v>
       </c>
       <c r="C84" s="5">
-        <v>0.28000000000000003</v>
+        <v>0.34</v>
       </c>
       <c r="E84" s="3">
         <v>14</v>
       </c>
       <c r="F84" s="4" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="G84" s="5">
-        <v>0.08</v>
+        <v>0.12</v>
       </c>
       <c r="I84" s="3">
         <v>14</v>
@@ -2964,16 +2964,16 @@
         <v>16</v>
       </c>
       <c r="K84" s="5">
-        <v>0.23</v>
+        <v>0.2</v>
       </c>
       <c r="M84" s="3">
         <v>14</v>
       </c>
       <c r="N84" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="O84" s="5">
-        <v>0.28000000000000003</v>
+        <v>0.28999999999999998</v>
       </c>
     </row>
     <row r="86" spans="1:15" x14ac:dyDescent="0.3">
@@ -3044,7 +3044,7 @@
         <v>10</v>
       </c>
       <c r="C88" s="3">
-        <v>11.5</v>
+        <v>10.7</v>
       </c>
       <c r="E88" s="3">
         <v>1</v>
@@ -3053,7 +3053,7 @@
         <v>13</v>
       </c>
       <c r="G88" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I88" s="3">
         <v>1</v>
@@ -3079,16 +3079,16 @@
         <v>2</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C89" s="3">
-        <v>11.5</v>
+        <v>12</v>
       </c>
       <c r="E89" s="3">
         <v>2</v>
       </c>
       <c r="F89" s="4" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="G89" s="3">
         <v>1</v>
@@ -3097,7 +3097,7 @@
         <v>2</v>
       </c>
       <c r="J89" s="4" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="K89" s="3">
         <v>3</v>
@@ -3106,7 +3106,7 @@
         <v>2</v>
       </c>
       <c r="N89" s="4" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="O89" s="3">
         <v>0</v>
@@ -3126,7 +3126,7 @@
         <v>3</v>
       </c>
       <c r="F90" s="4" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="G90" s="3">
         <v>1</v>
@@ -3135,7 +3135,7 @@
         <v>3</v>
       </c>
       <c r="J90" s="4" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="K90" s="3">
         <v>3</v>
@@ -3144,7 +3144,7 @@
         <v>3</v>
       </c>
       <c r="N90" s="4" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="O90" s="3">
         <v>0</v>
@@ -3155,16 +3155,16 @@
         <v>4</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C91" s="3">
-        <v>12.5</v>
+        <v>13</v>
       </c>
       <c r="E91" s="3">
         <v>4</v>
       </c>
       <c r="F91" s="4" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="G91" s="3">
         <v>1</v>
@@ -3193,16 +3193,16 @@
         <v>5</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C92" s="3">
-        <v>14</v>
+        <v>14.3</v>
       </c>
       <c r="E92" s="3">
         <v>5</v>
       </c>
       <c r="F92" s="4" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="G92" s="3">
         <v>1</v>
@@ -3231,16 +3231,16 @@
         <v>6</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C93" s="3">
-        <v>14</v>
+        <v>14.3</v>
       </c>
       <c r="E93" s="3">
         <v>6</v>
       </c>
       <c r="F93" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G93" s="3">
         <v>1</v>
@@ -3269,19 +3269,19 @@
         <v>7</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C94" s="3">
-        <v>14.5</v>
+        <v>15.5</v>
       </c>
       <c r="E94" s="3">
         <v>7</v>
       </c>
       <c r="F94" s="4" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G94" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I94" s="3">
         <v>7</v>
@@ -3307,25 +3307,25 @@
         <v>8</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C95" s="3">
-        <v>15.5</v>
+        <v>16</v>
       </c>
       <c r="E95" s="3">
         <v>8</v>
       </c>
       <c r="F95" s="4" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="G95" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I95" s="3">
         <v>8</v>
       </c>
       <c r="J95" s="4" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="K95" s="3">
         <v>1</v>
@@ -3334,7 +3334,7 @@
         <v>8</v>
       </c>
       <c r="N95" s="4" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="O95" s="3">
         <v>0</v>
@@ -3345,10 +3345,10 @@
         <v>9</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C96" s="3">
-        <v>16.5</v>
+        <v>16</v>
       </c>
       <c r="E96" s="3">
         <v>9</v>
@@ -3363,7 +3363,7 @@
         <v>9</v>
       </c>
       <c r="J96" s="4" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="K96" s="3">
         <v>1</v>
@@ -3372,7 +3372,7 @@
         <v>9</v>
       </c>
       <c r="N96" s="4" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="O96" s="3">
         <v>0</v>
@@ -3383,16 +3383,16 @@
         <v>10</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C97" s="3">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E97" s="3">
         <v>10</v>
       </c>
       <c r="F97" s="4" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="G97" s="3">
         <v>0</v>
@@ -3421,10 +3421,10 @@
         <v>11</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C98" s="3">
-        <v>17.5</v>
+        <v>16.7</v>
       </c>
       <c r="E98" s="3">
         <v>11</v>
@@ -3459,16 +3459,16 @@
         <v>12</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C99" s="3">
-        <v>18</v>
+        <v>17.3</v>
       </c>
       <c r="E99" s="3">
         <v>12</v>
       </c>
       <c r="F99" s="4" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="G99" s="3">
         <v>0</v>
@@ -3497,16 +3497,16 @@
         <v>13</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="C100" s="3">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E100" s="3">
         <v>13</v>
       </c>
       <c r="F100" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G100" s="3">
         <v>0</v>
@@ -3538,13 +3538,13 @@
         <v>11</v>
       </c>
       <c r="C101" s="3">
-        <v>22.5</v>
+        <v>20.3</v>
       </c>
       <c r="E101" s="3">
         <v>14</v>
       </c>
       <c r="F101" s="4" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="G101" s="3">
         <v>0</v>
@@ -3591,10 +3591,10 @@
         <v>1</v>
       </c>
       <c r="B105" s="4" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="C105" s="3">
-        <v>17</v>
+        <v>31</v>
       </c>
     </row>
     <row r="106" spans="1:15" x14ac:dyDescent="0.3">
@@ -3602,10 +3602,10 @@
         <v>2</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C106" s="3">
-        <v>20</v>
+        <v>35</v>
       </c>
     </row>
     <row r="107" spans="1:15" x14ac:dyDescent="0.3">
@@ -3613,10 +3613,10 @@
         <v>3</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C107" s="3">
-        <v>25</v>
+        <v>38</v>
       </c>
     </row>
     <row r="108" spans="1:15" x14ac:dyDescent="0.3">
@@ -3624,10 +3624,10 @@
         <v>4</v>
       </c>
       <c r="B108" s="4" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C108" s="3">
-        <v>26</v>
+        <v>40</v>
       </c>
     </row>
     <row r="109" spans="1:15" x14ac:dyDescent="0.3">
@@ -3635,10 +3635,10 @@
         <v>5</v>
       </c>
       <c r="B109" s="4" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C109" s="3">
-        <v>26</v>
+        <v>43</v>
       </c>
     </row>
     <row r="110" spans="1:15" x14ac:dyDescent="0.3">
@@ -3649,7 +3649,7 @@
         <v>6</v>
       </c>
       <c r="C110" s="3">
-        <v>31</v>
+        <v>45</v>
       </c>
     </row>
     <row r="111" spans="1:15" x14ac:dyDescent="0.3">
@@ -3657,10 +3657,10 @@
         <v>7</v>
       </c>
       <c r="B111" s="4" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C111" s="3">
-        <v>32</v>
+        <v>47</v>
       </c>
     </row>
     <row r="112" spans="1:15" x14ac:dyDescent="0.3">
@@ -3668,10 +3668,10 @@
         <v>8</v>
       </c>
       <c r="B112" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C112" s="3">
-        <v>33</v>
+        <v>50</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.3">
@@ -3679,10 +3679,10 @@
         <v>9</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C113" s="3">
-        <v>39</v>
+        <v>53</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.3">
@@ -3690,10 +3690,10 @@
         <v>10</v>
       </c>
       <c r="B114" s="4" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C114" s="3">
-        <v>39</v>
+        <v>54</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.3">
@@ -3701,10 +3701,10 @@
         <v>11</v>
       </c>
       <c r="B115" s="4" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C115" s="3">
-        <v>40</v>
+        <v>57</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.3">
@@ -3712,10 +3712,10 @@
         <v>12</v>
       </c>
       <c r="B116" s="4" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C116" s="3">
-        <v>41</v>
+        <v>57</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.3">
@@ -3723,10 +3723,10 @@
         <v>13</v>
       </c>
       <c r="B117" s="4" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C117" s="3">
-        <v>44</v>
+        <v>63</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.3">
@@ -3737,7 +3737,7 @@
         <v>11</v>
       </c>
       <c r="C118" s="3">
-        <v>48</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>